<commit_message>
ajout excell graphe cours
</commit_message>
<xml_diff>
--- a/Dijkstra4.xlsx
+++ b/Dijkstra4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\école\info ingé 2\projet S4\ReseauS4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C52B2BF6-CD1F-4371-979D-19EAD42EE6EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9316AAF-C5A3-4162-8DC2-BAF52B1A94A5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6870" yWindow="7845" windowWidth="21600" windowHeight="11385" xr2:uid="{42EF5A0C-F78C-417A-BA66-8C1B194455D2}"/>
+    <workbookView xWindow="4005" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{42EF5A0C-F78C-417A-BA66-8C1B194455D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>sommets</t>
   </si>
@@ -121,6 +121,27 @@
   </si>
   <si>
     <t>1-13-G</t>
+  </si>
+  <si>
+    <t>0-1-B</t>
+  </si>
+  <si>
+    <t>1-1-B</t>
+  </si>
+  <si>
+    <t>(0-2-D)</t>
+  </si>
+  <si>
+    <t>0-3-E</t>
+  </si>
+  <si>
+    <t>1-2-A/D</t>
+  </si>
+  <si>
+    <t>0-3-F</t>
+  </si>
+  <si>
+    <t>1-3-F/E</t>
   </si>
 </sst>
 </file>
@@ -136,7 +157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,6 +176,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -168,10 +195,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,15 +514,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4E578F-D4A1-496D-958E-54681DA4EDC4}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,8 +553,29 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -557,8 +606,29 @@
       <c r="J2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -571,8 +641,20 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -586,8 +668,21 @@
       <c r="I4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="3"/>
+      <c r="O4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -599,8 +694,19 @@
       <c r="J5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="P5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -616,8 +722,20 @@
       <c r="H6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -628,8 +746,21 @@
       <c r="J7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -644,8 +775,19 @@
         <v>25</v>
       </c>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" t="s">
+        <v>36</v>
+      </c>
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -658,8 +800,17 @@
         <v>28</v>
       </c>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>7</v>
+      </c>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -673,8 +824,17 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -689,8 +849,17 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>9</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -703,8 +872,17 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -717,8 +895,17 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>11</v>
+      </c>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -731,8 +918,17 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>12</v>
+      </c>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -745,8 +941,17 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>13</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -759,8 +964,17 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>14</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -773,11 +987,21 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>15</v>
+      </c>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>